<commit_message>
New tag get all endpoint was implemented
</commit_message>
<xml_diff>
--- a/src/main/resources/words.xlsx
+++ b/src/main/resources/words.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
   <si>
     <t>contrived</t>
   </si>
@@ -210,6 +210,21 @@
   <si>
     <t>İlgili, uygun</t>
   </si>
+  <si>
+    <t>allude</t>
+  </si>
+  <si>
+    <t>İma etmek, kast etmek, üstü kapalı söylemek</t>
+  </si>
+  <si>
+    <t>regress</t>
+  </si>
+  <si>
+    <t>bears</t>
+  </si>
+  <si>
+    <t>Taşımak, katlanmak</t>
+  </si>
 </sst>
 </file>
 
@@ -251,12 +266,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -269,16 +290,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -295,25 +316,25 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -334,6 +355,7 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffea4335"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -533,12 +555,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -571,10 +593,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -822,12 +844,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1142,10 +1164,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1614,7 +1636,7 @@
         <v>35</v>
       </c>
       <c r="C16" t="s" s="4">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1815,23 +1837,41 @@
       <c r="E31" s="5"/>
     </row>
     <row r="32" ht="23.4" customHeight="1">
-      <c r="A32" s="6"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
+      <c r="A32" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="B32" t="s" s="3">
+        <v>67</v>
+      </c>
+      <c r="C32" t="s" s="4">
+        <v>12</v>
+      </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
     </row>
     <row r="33" ht="23.4" customHeight="1">
-      <c r="A33" s="6"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
+      <c r="A33" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="B33" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s" s="4">
+        <v>12</v>
+      </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
     </row>
     <row r="34" ht="23.4" customHeight="1">
-      <c r="A34" s="6"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="8"/>
+      <c r="A34" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="B34" t="s" s="3">
+        <v>70</v>
+      </c>
+      <c r="C34" t="s" s="4">
+        <v>12</v>
+      </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>

</xml_diff>

<commit_message>
datamodel implemented with graph data model
</commit_message>
<xml_diff>
--- a/src/main/resources/words.xlsx
+++ b/src/main/resources/words.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="72">
   <si>
     <t xml:space="preserve">contrived</t>
   </si>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">competency</t>
   </si>
   <si>
-    <t xml:space="preserve">güç, yetekenek, ehliyet</t>
+    <t xml:space="preserve">ehliyet, yetki, yeterlilik, güç</t>
   </si>
   <si>
     <t xml:space="preserve">adhere</t>
@@ -140,9 +140,6 @@
   </si>
   <si>
     <t xml:space="preserve">sıkı, zorlayıcı, bağlayıcı</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yetkinlik, güç, ehliyet</t>
   </si>
   <si>
     <t xml:space="preserve">reason out</t>
@@ -396,20 +393,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="86.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="86.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="1" width="12.67"/>
   </cols>
   <sheetData>
@@ -649,75 +646,75 @@
     </row>
     <row r="19" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>12</v>
@@ -727,49 +724,49 @@
     </row>
     <row r="25" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>5</v>
@@ -779,49 +776,49 @@
     </row>
     <row r="29" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>12</v>
@@ -834,7 +831,7 @@
         <v>68</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>12</v>
@@ -843,28 +840,22 @@
       <c r="E33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34" s="3" t="s">
+      <c r="A34" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="B34" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="A35" s="6"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="8"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
     </row>
@@ -7616,13 +7607,7 @@
       <c r="D999" s="5"/>
       <c r="E999" s="5"/>
     </row>
-    <row r="1000" customFormat="false" ht="23.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1000" s="6"/>
-      <c r="B1000" s="7"/>
-      <c r="C1000" s="8"/>
-      <c r="D1000" s="5"/>
-      <c r="E1000" s="5"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.511811023622047" footer="0.25"/>

</xml_diff>